<commit_message>
Update test files for PPTX and XLSX formats to reflect recent changes and added an app
</commit_message>
<xml_diff>
--- a/tests/sheet_test/test_sheet.xlsx
+++ b/tests/sheet_test/test_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tariq\Desktop\ppt-automate\sheet_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tariq\Desktop\ppt-automate\tests\sheet_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA34FD44-EA80-433C-887E-C1495A84D51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77D3A9E-EFFE-4CF1-B3D3-A4FB4E855BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E47A7D9-A4BB-4162-BB07-162114737A56}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{1E47A7D9-A4BB-4162-BB07-162114737A56}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>DR</t>
   </si>
@@ -108,13 +108,16 @@
   </si>
   <si>
     <t>PERCENT</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,7 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -208,24 +211,100 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="11">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Aptos"/>
+        <color theme="1"/>
+        <name val="Abadi Extra Light"/>
         <family val="2"/>
         <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Abadi Extra Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Abadi Extra Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Abadi Extra Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
       </font>
     </dxf>
     <dxf>
@@ -307,17 +386,16 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
     </dxf>
   </dxfs>
@@ -1291,16 +1369,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>713247</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>170119</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>530367</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>162720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1329,17 +1407,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0832E61-E343-4084-B153-C849BB92A182}" name="Tableau1" displayName="Tableau1" ref="A1:D11" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0832E61-E343-4084-B153-C849BB92A182}" name="Tableau1" displayName="Tableau1" ref="A1:D12" totalsRowCount="1" headerRowDxfId="10">
   <autoFilter ref="A1:D11" xr:uid="{D0832E61-E343-4084-B153-C849BB92A182}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A5E19816-F8B1-45CA-886D-F7FB6844A67E}" name="DR" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{21946E90-0BAB-4D61-A1DB-8B1F8707D778}" name="MOIS" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{41012845-28F3-4C5C-9E65-AFC59D1FE544}" name="VALUE" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{17A2E0B4-52B5-45C0-856E-82BF92DFAD1F}" name="PERCENT" dataDxfId="1" dataCellStyle="Pourcentage">
-      <calculatedColumnFormula>C2/$C$13</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{A5E19816-F8B1-45CA-886D-F7FB6844A67E}" name="DR" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{21946E90-0BAB-4D61-A1DB-8B1F8707D778}" name="MOIS" dataDxfId="8" totalsRowDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{41012845-28F3-4C5C-9E65-AFC59D1FE544}" name="VALUE" dataDxfId="7" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{17A2E0B4-52B5-45C0-856E-82BF92DFAD1F}" name="PERCENT" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="0" dataCellStyle="Pourcentage">
+      <calculatedColumnFormula>C2/$H$1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1661,15 +1739,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56520370-808B-4451-981E-17803BF508AD}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="C6" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1682,8 +1760,10 @@
       <c r="D1" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1693,12 +1773,12 @@
       <c r="C2" s="4">
         <v>5</v>
       </c>
-      <c r="D2" s="6">
-        <f>C2/$C$13</f>
-        <v>3.5360678925035359E-3</v>
+      <c r="D2" s="6" t="e">
+        <f t="shared" ref="D2:D11" si="0">C2/$H$1</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1708,12 +1788,12 @@
       <c r="C3" s="4">
         <v>18</v>
       </c>
-      <c r="D3" s="6">
-        <f t="shared" ref="D3:D11" si="0">C3/$C$13</f>
-        <v>1.272984441301273E-2</v>
+      <c r="D3" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1723,12 +1803,12 @@
       <c r="C4" s="4">
         <v>451</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="6" t="e">
         <f t="shared" si="0"/>
-        <v>0.31895332390381897</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1738,12 +1818,12 @@
       <c r="C5" s="4">
         <v>100</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="6" t="e">
         <f t="shared" si="0"/>
-        <v>7.0721357850070721E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1753,12 +1833,12 @@
       <c r="C6" s="4">
         <v>50</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="6" t="e">
         <f t="shared" si="0"/>
-        <v>3.536067892503536E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1768,12 +1848,12 @@
       <c r="C7" s="4">
         <v>123</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="6" t="e">
         <f t="shared" si="0"/>
-        <v>8.6987270155586993E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1783,12 +1863,12 @@
       <c r="C8" s="4">
         <v>11</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="6" t="e">
         <f t="shared" si="0"/>
-        <v>7.7793493635077791E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1798,12 +1878,12 @@
       <c r="C9" s="4">
         <v>16</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="6" t="e">
         <f t="shared" si="0"/>
-        <v>1.1315417256011316E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1813,12 +1893,12 @@
       <c r="C10" s="4">
         <v>500</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="6" t="e">
         <f t="shared" si="0"/>
-        <v>0.3536067892503536</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -1828,31 +1908,32 @@
       <c r="C11" s="4">
         <v>140</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="6" t="e">
         <f t="shared" si="0"/>
-        <v>9.9009900990099015E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
+    <row r="12" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="8">
+        <f>SUBTOTAL(103,Tableau1[PERCENT])</f>
+        <v>10</v>
+      </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="3">
-        <f>(C11/C13)</f>
-        <v>9.9009900990099015E-2</v>
-      </c>
-      <c r="C13" s="2">
-        <f>SUM(C2:C11)</f>
-        <v>1414</v>
-      </c>
+    <row r="13" spans="1:8">
+      <c r="B13" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>